<commit_message>
adding results for overall analysis, but still need to write it into a function
</commit_message>
<xml_diff>
--- a/3_Results/32_ResultsVMMC/vmmc_individual_adjusted.xlsx
+++ b/3_Results/32_ResultsVMMC/vmmc_individual_adjusted.xlsx
@@ -553,28 +553,28 @@
         </is>
       </c>
       <c r="D2">
-        <v>-1.139</v>
+        <v>-1.14</v>
       </c>
       <c r="E2">
-        <v>-2.109</v>
+        <v>-2.11</v>
       </c>
       <c r="F2">
-        <v>-0.168</v>
+        <v>-0.17</v>
       </c>
       <c r="G2">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="H2">
-        <v>0.245</v>
+        <v>0.25</v>
       </c>
       <c r="I2">
-        <v>0.495</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GLMM</t>
+          <t>GLM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -584,35 +584,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D3">
-        <v>-1.139</v>
+        <v>-0.11</v>
       </c>
       <c r="E3">
-        <v>-2.109</v>
+        <v>-1.5</v>
       </c>
       <c r="F3">
-        <v>-0.169</v>
+        <v>1.28</v>
       </c>
       <c r="G3">
-        <v>0.021</v>
+        <v>0.88</v>
       </c>
       <c r="H3">
-        <v>0.245</v>
+        <v>0.5</v>
       </c>
       <c r="I3">
-        <v>0.495</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GEE</t>
+          <t>GLM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -622,29 +619,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect Calculated</t>
         </is>
       </c>
       <c r="D4">
-        <v>-1.068</v>
-      </c>
-      <c r="E4">
-        <v>-1.928</v>
-      </c>
-      <c r="F4">
-        <v>-0.207</v>
-      </c>
-      <c r="G4">
-        <v>0.015</v>
-      </c>
-      <c r="H4">
-        <v>0.193</v>
-      </c>
-      <c r="I4">
-        <v>0.439</v>
-      </c>
-      <c r="J4">
-        <v>-0.003</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="5">
@@ -660,32 +639,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D5">
-        <v>-0.109</v>
+        <v>-1.25</v>
       </c>
       <c r="E5">
-        <v>-1.5</v>
+        <v>-2.21</v>
       </c>
       <c r="F5">
-        <v>1.283</v>
+        <v>-0.28</v>
       </c>
       <c r="G5">
-        <v>0.878</v>
+        <v>0.01</v>
       </c>
       <c r="H5">
-        <v>0.504</v>
+        <v>0.24</v>
       </c>
       <c r="I5">
-        <v>0.71</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GLMM</t>
+          <t>GLM</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -695,32 +674,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D6">
-        <v>-0.109</v>
+        <v>0.09</v>
       </c>
       <c r="E6">
-        <v>-1.476</v>
+        <v>-0.98</v>
       </c>
       <c r="F6">
-        <v>1.259</v>
+        <v>1.16</v>
       </c>
       <c r="G6">
-        <v>0.876</v>
+        <v>0.44</v>
       </c>
       <c r="H6">
-        <v>0.487</v>
+        <v>0.3</v>
       </c>
       <c r="I6">
-        <v>0.698</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GEE</t>
+          <t>GLM</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -730,32 +709,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>PM Calculated</t>
         </is>
       </c>
       <c r="D7">
-        <v>-0.054</v>
-      </c>
-      <c r="E7">
-        <v>-1.252</v>
-      </c>
-      <c r="F7">
-        <v>1.145</v>
-      </c>
-      <c r="G7">
-        <v>0.93</v>
-      </c>
-      <c r="H7">
-        <v>0.374</v>
-      </c>
-      <c r="I7">
-        <v>0.612</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GLM</t>
+          <t>GLMM</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -765,11 +729,29 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Indirect Calculated</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D8">
-        <v>-0.109</v>
+        <v>-1.14</v>
+      </c>
+      <c r="E8">
+        <v>-2.11</v>
+      </c>
+      <c r="F8">
+        <v>-0.17</v>
+      </c>
+      <c r="G8">
+        <v>0.02</v>
+      </c>
+      <c r="H8">
+        <v>0.24</v>
+      </c>
+      <c r="I8">
+        <v>0.49</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -785,17 +767,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Indirect Calculated</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D9">
-        <v>-0.109</v>
+        <v>-0.11</v>
+      </c>
+      <c r="E9">
+        <v>-1.48</v>
+      </c>
+      <c r="F9">
+        <v>1.26</v>
+      </c>
+      <c r="G9">
+        <v>0.88</v>
+      </c>
+      <c r="H9">
+        <v>0.49</v>
+      </c>
+      <c r="I9">
+        <v>0.7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GEE</t>
+          <t>GLMM</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -809,13 +806,13 @@
         </is>
       </c>
       <c r="D10">
-        <v>-0.059</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GLM</t>
+          <t>GLMM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -829,22 +826,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>-1.247</v>
+        <v>-1.25</v>
       </c>
       <c r="E11">
-        <v>-2.212</v>
+        <v>-2.21</v>
       </c>
       <c r="F11">
-        <v>-0.283</v>
+        <v>-0.28</v>
       </c>
       <c r="G11">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="H11">
-        <v>0.242</v>
+        <v>0.24</v>
       </c>
       <c r="I11">
-        <v>0.492</v>
+        <v>0.49</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -860,35 +860,32 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D12">
-        <v>-1.247</v>
+        <v>0.09</v>
       </c>
       <c r="E12">
-        <v>-2.212</v>
+        <v>-0.96</v>
       </c>
       <c r="F12">
-        <v>-0.283</v>
+        <v>1.14</v>
       </c>
       <c r="G12">
-        <v>0.011</v>
+        <v>0.44</v>
       </c>
       <c r="H12">
-        <v>0.242</v>
+        <v>0.29</v>
       </c>
       <c r="I12">
-        <v>0.492</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GEE</t>
+          <t>GLMM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -898,35 +895,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>PM Calculated</t>
         </is>
       </c>
       <c r="D13">
-        <v>-1.126</v>
-      </c>
-      <c r="E13">
-        <v>-1.96</v>
-      </c>
-      <c r="F13">
-        <v>-0.293</v>
-      </c>
-      <c r="G13">
-        <v>0.008</v>
-      </c>
-      <c r="H13">
-        <v>0.181</v>
-      </c>
-      <c r="I13">
-        <v>0.425</v>
-      </c>
-      <c r="J13">
-        <v>-0.003</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GLM</t>
+          <t>GEE</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -936,32 +915,35 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D14">
-        <v>0.08699999999999999</v>
+        <v>-1.07</v>
       </c>
       <c r="E14">
-        <v>-0.982</v>
+        <v>-1.93</v>
       </c>
       <c r="F14">
-        <v>1.157</v>
+        <v>-0.21</v>
       </c>
       <c r="G14">
-        <v>0.437</v>
+        <v>0.02</v>
       </c>
       <c r="H14">
-        <v>0.298</v>
+        <v>0.19</v>
       </c>
       <c r="I14">
-        <v>0.546</v>
+        <v>0.44</v>
+      </c>
+      <c r="J14">
+        <v>-0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GLMM</t>
+          <t>GEE</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -971,26 +953,26 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D15">
-        <v>0.08699999999999999</v>
+        <v>-0.05</v>
       </c>
       <c r="E15">
-        <v>-0.963</v>
+        <v>-1.25</v>
       </c>
       <c r="F15">
-        <v>1.137</v>
+        <v>1.14</v>
       </c>
       <c r="G15">
-        <v>0.435</v>
+        <v>0.93</v>
       </c>
       <c r="H15">
-        <v>0.287</v>
+        <v>0.37</v>
       </c>
       <c r="I15">
-        <v>0.536</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="16">
@@ -1006,32 +988,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Indirect Calculated</t>
         </is>
       </c>
       <c r="D16">
-        <v>0.048</v>
-      </c>
-      <c r="E16">
-        <v>-0.995</v>
-      </c>
-      <c r="F16">
-        <v>1.09</v>
-      </c>
-      <c r="G16">
-        <v>0.464</v>
-      </c>
-      <c r="H16">
-        <v>0.283</v>
-      </c>
-      <c r="I16">
-        <v>0.532</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GLM</t>
+          <t>GEE</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1041,17 +1008,35 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>PM Calculated</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D17">
-        <v>0.08699999999999999</v>
+        <v>-1.13</v>
+      </c>
+      <c r="E17">
+        <v>-1.96</v>
+      </c>
+      <c r="F17">
+        <v>-0.29</v>
+      </c>
+      <c r="G17">
+        <v>0.01</v>
+      </c>
+      <c r="H17">
+        <v>0.18</v>
+      </c>
+      <c r="I17">
+        <v>0.43</v>
+      </c>
+      <c r="J17">
+        <v>-0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GLMM</t>
+          <t>GEE</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1061,11 +1046,26 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>PM Calculated</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D18">
-        <v>0.08699999999999999</v>
+        <v>0.05</v>
+      </c>
+      <c r="E18">
+        <v>-1</v>
+      </c>
+      <c r="F18">
+        <v>1.09</v>
+      </c>
+      <c r="G18">
+        <v>0.46</v>
+      </c>
+      <c r="H18">
+        <v>0.28</v>
+      </c>
+      <c r="I18">
+        <v>0.53</v>
       </c>
     </row>
     <row r="19">
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="D19">
-        <v>0.052</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -1173,25 +1173,25 @@
         <v>0.32</v>
       </c>
       <c r="E2">
-        <v>0.121</v>
+        <v>0.12</v>
       </c>
       <c r="F2">
-        <v>0.845</v>
+        <v>0.85</v>
       </c>
       <c r="G2">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="H2">
-        <v>0.245</v>
+        <v>0.25</v>
       </c>
       <c r="I2">
-        <v>0.495</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GLMM</t>
+          <t>GLM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1201,35 +1201,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D3">
-        <v>0.32</v>
+        <v>0.9</v>
       </c>
       <c r="E3">
-        <v>0.121</v>
+        <v>0.22</v>
       </c>
       <c r="F3">
-        <v>0.845</v>
+        <v>3.61</v>
       </c>
       <c r="G3">
-        <v>0.021</v>
+        <v>0.88</v>
       </c>
       <c r="H3">
-        <v>0.245</v>
+        <v>0.5</v>
       </c>
       <c r="I3">
-        <v>0.495</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GEE</t>
+          <t>GLM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1239,29 +1236,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect Calculated</t>
         </is>
       </c>
       <c r="D4">
-        <v>0.344</v>
-      </c>
-      <c r="E4">
-        <v>0.145</v>
-      </c>
-      <c r="F4">
-        <v>0.8129999999999999</v>
-      </c>
-      <c r="G4">
-        <v>0.015</v>
-      </c>
-      <c r="H4">
-        <v>0.193</v>
-      </c>
-      <c r="I4">
-        <v>0.439</v>
-      </c>
-      <c r="J4">
-        <v>-0.003</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5">
@@ -1277,32 +1256,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D5">
-        <v>0.897</v>
+        <v>0.29</v>
       </c>
       <c r="E5">
-        <v>0.223</v>
+        <v>0.11</v>
       </c>
       <c r="F5">
-        <v>3.607</v>
+        <v>0.75</v>
       </c>
       <c r="G5">
-        <v>0.878</v>
+        <v>0.01</v>
       </c>
       <c r="H5">
-        <v>0.504</v>
+        <v>0.24</v>
       </c>
       <c r="I5">
-        <v>0.71</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GLMM</t>
+          <t>GLM</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1312,32 +1291,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D6">
-        <v>0.897</v>
+        <v>0.09</v>
       </c>
       <c r="E6">
-        <v>0.228</v>
+        <v>-0.98</v>
       </c>
       <c r="F6">
-        <v>3.522</v>
+        <v>1.16</v>
       </c>
       <c r="G6">
-        <v>0.876</v>
+        <v>0.44</v>
       </c>
       <c r="H6">
-        <v>0.487</v>
+        <v>0.3</v>
       </c>
       <c r="I6">
-        <v>0.698</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GEE</t>
+          <t>GLM</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1347,32 +1326,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>PM Calculated</t>
         </is>
       </c>
       <c r="D7">
-        <v>0.948</v>
-      </c>
-      <c r="E7">
-        <v>0.286</v>
-      </c>
-      <c r="F7">
-        <v>3.142</v>
-      </c>
-      <c r="G7">
-        <v>0.93</v>
-      </c>
-      <c r="H7">
-        <v>0.374</v>
-      </c>
-      <c r="I7">
-        <v>0.612</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GLM</t>
+          <t>GLMM</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1382,11 +1346,29 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Indirect Calculated</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D8">
-        <v>0.897</v>
+        <v>0.32</v>
+      </c>
+      <c r="E8">
+        <v>0.12</v>
+      </c>
+      <c r="F8">
+        <v>0.84</v>
+      </c>
+      <c r="G8">
+        <v>0.02</v>
+      </c>
+      <c r="H8">
+        <v>0.24</v>
+      </c>
+      <c r="I8">
+        <v>0.49</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1402,17 +1384,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Indirect Calculated</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D9">
-        <v>0.897</v>
+        <v>0.9</v>
+      </c>
+      <c r="E9">
+        <v>0.23</v>
+      </c>
+      <c r="F9">
+        <v>3.52</v>
+      </c>
+      <c r="G9">
+        <v>0.88</v>
+      </c>
+      <c r="H9">
+        <v>0.49</v>
+      </c>
+      <c r="I9">
+        <v>0.7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GEE</t>
+          <t>GLMM</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1426,13 +1423,13 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.9429999999999999</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GLM</t>
+          <t>GLMM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1446,22 +1443,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.287</v>
+        <v>0.29</v>
       </c>
       <c r="E11">
-        <v>0.109</v>
+        <v>0.11</v>
       </c>
       <c r="F11">
-        <v>0.753</v>
+        <v>0.75</v>
       </c>
       <c r="G11">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="H11">
-        <v>0.242</v>
+        <v>0.24</v>
       </c>
       <c r="I11">
-        <v>0.492</v>
+        <v>0.49</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1477,35 +1477,32 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D12">
-        <v>0.287</v>
+        <v>0.09</v>
       </c>
       <c r="E12">
-        <v>0.11</v>
+        <v>-0.96</v>
       </c>
       <c r="F12">
-        <v>0.753</v>
+        <v>1.14</v>
       </c>
       <c r="G12">
-        <v>0.011</v>
+        <v>0.44</v>
       </c>
       <c r="H12">
-        <v>0.242</v>
+        <v>0.29</v>
       </c>
       <c r="I12">
-        <v>0.492</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GEE</t>
+          <t>GLMM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1515,35 +1512,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>PM Calculated</t>
         </is>
       </c>
       <c r="D13">
-        <v>0.324</v>
-      </c>
-      <c r="E13">
-        <v>0.141</v>
-      </c>
-      <c r="F13">
-        <v>0.746</v>
-      </c>
-      <c r="G13">
-        <v>0.008</v>
-      </c>
-      <c r="H13">
-        <v>0.181</v>
-      </c>
-      <c r="I13">
-        <v>0.425</v>
-      </c>
-      <c r="J13">
-        <v>-0.003</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GLM</t>
+          <t>GEE</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1553,32 +1532,35 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D14">
-        <v>0.08699999999999999</v>
+        <v>0.34</v>
       </c>
       <c r="E14">
-        <v>-0.982</v>
+        <v>0.15</v>
       </c>
       <c r="F14">
-        <v>1.157</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="G14">
-        <v>0.437</v>
+        <v>0.02</v>
       </c>
       <c r="H14">
-        <v>0.298</v>
+        <v>0.19</v>
       </c>
       <c r="I14">
-        <v>0.546</v>
+        <v>0.44</v>
+      </c>
+      <c r="J14">
+        <v>-0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GLMM</t>
+          <t>GEE</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1588,26 +1570,26 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D15">
-        <v>0.08699999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="E15">
-        <v>-0.963</v>
+        <v>0.29</v>
       </c>
       <c r="F15">
-        <v>1.137</v>
+        <v>3.14</v>
       </c>
       <c r="G15">
-        <v>0.435</v>
+        <v>0.93</v>
       </c>
       <c r="H15">
-        <v>0.287</v>
+        <v>0.37</v>
       </c>
       <c r="I15">
-        <v>0.536</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="16">
@@ -1623,32 +1605,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Indirect Calculated</t>
         </is>
       </c>
       <c r="D16">
-        <v>0.048</v>
-      </c>
-      <c r="E16">
-        <v>-0.995</v>
-      </c>
-      <c r="F16">
-        <v>1.09</v>
-      </c>
-      <c r="G16">
-        <v>0.464</v>
-      </c>
-      <c r="H16">
-        <v>0.283</v>
-      </c>
-      <c r="I16">
-        <v>0.532</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GLM</t>
+          <t>GEE</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1658,17 +1625,35 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>PM Calculated</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D17">
-        <v>0.08699999999999999</v>
+        <v>0.32</v>
+      </c>
+      <c r="E17">
+        <v>0.14</v>
+      </c>
+      <c r="F17">
+        <v>0.75</v>
+      </c>
+      <c r="G17">
+        <v>0.01</v>
+      </c>
+      <c r="H17">
+        <v>0.18</v>
+      </c>
+      <c r="I17">
+        <v>0.43</v>
+      </c>
+      <c r="J17">
+        <v>-0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GLMM</t>
+          <t>GEE</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1678,11 +1663,26 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>PM Calculated</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D18">
-        <v>0.08699999999999999</v>
+        <v>0.05</v>
+      </c>
+      <c r="E18">
+        <v>-1</v>
+      </c>
+      <c r="F18">
+        <v>1.09</v>
+      </c>
+      <c r="G18">
+        <v>0.46</v>
+      </c>
+      <c r="H18">
+        <v>0.28</v>
+      </c>
+      <c r="I18">
+        <v>0.53</v>
       </c>
     </row>
     <row r="19">
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="D19">
-        <v>0.052</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -1787,22 +1787,22 @@
         </is>
       </c>
       <c r="D2">
-        <v>-1.247</v>
+        <v>-1.25</v>
       </c>
       <c r="E2">
-        <v>-2.212</v>
+        <v>-2.21</v>
       </c>
       <c r="F2">
-        <v>-0.283</v>
+        <v>-0.28</v>
       </c>
       <c r="G2">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="H2">
-        <v>0.242</v>
+        <v>0.24</v>
       </c>
       <c r="I2">
-        <v>0.492</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="3">
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="D3">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
       <c r="E3">
         <v>-0.04</v>
@@ -1831,13 +1831,13 @@
         <v>0.05</v>
       </c>
       <c r="G3">
-        <v>0.822</v>
+        <v>0.82</v>
       </c>
       <c r="H3">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4">
@@ -1866,13 +1866,13 @@
         <v>0.83</v>
       </c>
       <c r="G4">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="H4">
-        <v>0.034</v>
+        <v>0.03</v>
       </c>
       <c r="I4">
-        <v>0.184</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="5">
@@ -1892,22 +1892,22 @@
         </is>
       </c>
       <c r="D5">
-        <v>5.298</v>
+        <v>5.3</v>
       </c>
       <c r="E5">
-        <v>-2.336</v>
+        <v>-2.34</v>
       </c>
       <c r="F5">
-        <v>12.933</v>
+        <v>12.93</v>
       </c>
       <c r="G5">
-        <v>0.174</v>
+        <v>0.17</v>
       </c>
       <c r="H5">
-        <v>15.172</v>
+        <v>15.17</v>
       </c>
       <c r="I5">
-        <v>3.895</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="6">
@@ -1927,22 +1927,22 @@
         </is>
       </c>
       <c r="D6">
-        <v>6.478</v>
+        <v>6.48</v>
       </c>
       <c r="E6">
-        <v>-11.159</v>
+        <v>-11.16</v>
       </c>
       <c r="F6">
-        <v>24.114</v>
+        <v>24.11</v>
       </c>
       <c r="G6">
-        <v>0.472</v>
+        <v>0.47</v>
       </c>
       <c r="H6">
-        <v>80.97199999999999</v>
+        <v>80.97</v>
       </c>
       <c r="I6">
-        <v>8.997999999999999</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -1962,22 +1962,22 @@
         </is>
       </c>
       <c r="D7">
-        <v>4.901</v>
+        <v>4.9</v>
       </c>
       <c r="E7">
-        <v>-3.457</v>
+        <v>-3.46</v>
       </c>
       <c r="F7">
-        <v>13.258</v>
+        <v>13.26</v>
       </c>
       <c r="G7">
         <v>0.25</v>
       </c>
       <c r="H7">
-        <v>18.181</v>
+        <v>18.18</v>
       </c>
       <c r="I7">
-        <v>4.264</v>
+        <v>4.26</v>
       </c>
     </row>
     <row r="8">
@@ -1997,22 +1997,22 @@
         </is>
       </c>
       <c r="D8">
-        <v>-1.247</v>
+        <v>-1.25</v>
       </c>
       <c r="E8">
-        <v>-2.212</v>
+        <v>-2.21</v>
       </c>
       <c r="F8">
-        <v>-0.283</v>
+        <v>-0.28</v>
       </c>
       <c r="G8">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="H8">
-        <v>0.242</v>
+        <v>0.24</v>
       </c>
       <c r="I8">
-        <v>0.492</v>
+        <v>0.49</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -2035,7 +2035,7 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
       <c r="E9">
         <v>-0.04</v>
@@ -2044,13 +2044,13 @@
         <v>0.05</v>
       </c>
       <c r="G9">
-        <v>0.822</v>
+        <v>0.82</v>
       </c>
       <c r="H9">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -2082,13 +2082,13 @@
         <v>0.83</v>
       </c>
       <c r="G10">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="H10">
-        <v>0.034</v>
+        <v>0.03</v>
       </c>
       <c r="I10">
-        <v>0.184</v>
+        <v>0.18</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -2111,22 +2111,22 @@
         </is>
       </c>
       <c r="D11">
-        <v>5.298</v>
+        <v>5.3</v>
       </c>
       <c r="E11">
-        <v>-2.332</v>
+        <v>-2.33</v>
       </c>
       <c r="F11">
-        <v>12.928</v>
+        <v>12.93</v>
       </c>
       <c r="G11">
-        <v>0.174</v>
+        <v>0.17</v>
       </c>
       <c r="H11">
-        <v>15.154</v>
+        <v>15.15</v>
       </c>
       <c r="I11">
-        <v>3.893</v>
+        <v>3.89</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2149,22 +2149,22 @@
         </is>
       </c>
       <c r="D12">
-        <v>6.478</v>
+        <v>6.48</v>
       </c>
       <c r="E12">
-        <v>-11.134</v>
+        <v>-11.13</v>
       </c>
       <c r="F12">
         <v>24.09</v>
       </c>
       <c r="G12">
-        <v>0.471</v>
+        <v>0.47</v>
       </c>
       <c r="H12">
-        <v>80.748</v>
+        <v>80.75</v>
       </c>
       <c r="I12">
-        <v>8.986000000000001</v>
+        <v>8.99</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -2187,13 +2187,13 @@
         </is>
       </c>
       <c r="D13">
-        <v>4.901</v>
+        <v>4.9</v>
       </c>
       <c r="E13">
-        <v>-3.452</v>
+        <v>-3.45</v>
       </c>
       <c r="F13">
-        <v>13.253</v>
+        <v>13.25</v>
       </c>
       <c r="G13">
         <v>0.25</v>
@@ -2202,7 +2202,7 @@
         <v>18.16</v>
       </c>
       <c r="I13">
-        <v>4.261</v>
+        <v>4.26</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -2225,25 +2225,25 @@
         </is>
       </c>
       <c r="D14">
-        <v>-1.126</v>
+        <v>-1.13</v>
       </c>
       <c r="E14">
         <v>-1.96</v>
       </c>
       <c r="F14">
-        <v>-0.293</v>
+        <v>-0.29</v>
       </c>
       <c r="G14">
-        <v>0.008</v>
+        <v>0.01</v>
       </c>
       <c r="H14">
-        <v>0.181</v>
+        <v>0.18</v>
       </c>
       <c r="I14">
-        <v>0.425</v>
+        <v>0.43</v>
       </c>
       <c r="J14">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="15">
@@ -2263,25 +2263,25 @@
         </is>
       </c>
       <c r="D15">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>-0.027</v>
+        <v>-0.03</v>
       </c>
       <c r="F15">
-        <v>0.037</v>
+        <v>0.04</v>
       </c>
       <c r="G15">
-        <v>0.757</v>
+        <v>0.76</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0.016</v>
+        <v>0.02</v>
       </c>
       <c r="J15">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="16">
@@ -2301,25 +2301,25 @@
         </is>
       </c>
       <c r="D16">
-        <v>0.458</v>
+        <v>0.46</v>
       </c>
       <c r="E16">
-        <v>0.162</v>
+        <v>0.16</v>
       </c>
       <c r="F16">
-        <v>0.754</v>
+        <v>0.75</v>
       </c>
       <c r="G16">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
       <c r="I16">
-        <v>0.151</v>
+        <v>0.15</v>
       </c>
       <c r="J16">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="17">
@@ -2342,10 +2342,10 @@
         <v>5.94</v>
       </c>
       <c r="E17">
-        <v>0.928</v>
+        <v>0.93</v>
       </c>
       <c r="F17">
-        <v>10.952</v>
+        <v>10.95</v>
       </c>
       <c r="G17">
         <v>0.02</v>
@@ -2354,10 +2354,10 @@
         <v>6.54</v>
       </c>
       <c r="I17">
-        <v>2.557</v>
+        <v>2.56</v>
       </c>
       <c r="J17">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="18">
@@ -2377,25 +2377,25 @@
         </is>
       </c>
       <c r="D18">
-        <v>5.186</v>
+        <v>5.19</v>
       </c>
       <c r="E18">
         <v>-10.56</v>
       </c>
       <c r="F18">
-        <v>20.932</v>
+        <v>20.93</v>
       </c>
       <c r="G18">
-        <v>0.519</v>
+        <v>0.52</v>
       </c>
       <c r="H18">
-        <v>64.54300000000001</v>
+        <v>64.54000000000001</v>
       </c>
       <c r="I18">
-        <v>8.034000000000001</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="J18">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="19">
@@ -2415,25 +2415,25 @@
         </is>
       </c>
       <c r="D19">
-        <v>4.176</v>
+        <v>4.18</v>
       </c>
       <c r="E19">
-        <v>-2.629</v>
+        <v>-2.63</v>
       </c>
       <c r="F19">
-        <v>10.981</v>
+        <v>10.98</v>
       </c>
       <c r="G19">
-        <v>0.229</v>
+        <v>0.23</v>
       </c>
       <c r="H19">
-        <v>12.054</v>
+        <v>12.05</v>
       </c>
       <c r="I19">
-        <v>3.472</v>
+        <v>3.47</v>
       </c>
       <c r="J19">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
   </sheetData>
@@ -2518,22 +2518,22 @@
         </is>
       </c>
       <c r="D2">
-        <v>0.287</v>
+        <v>0.29</v>
       </c>
       <c r="E2">
-        <v>0.109</v>
+        <v>0.11</v>
       </c>
       <c r="F2">
-        <v>0.753</v>
+        <v>0.75</v>
       </c>
       <c r="G2">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="H2">
-        <v>0.242</v>
+        <v>0.24</v>
       </c>
       <c r="I2">
-        <v>0.492</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="3">
@@ -2553,22 +2553,22 @@
         </is>
       </c>
       <c r="D3">
-        <v>1.005</v>
+        <v>1.01</v>
       </c>
       <c r="E3">
-        <v>0.961</v>
+        <v>0.96</v>
       </c>
       <c r="F3">
-        <v>1.052</v>
+        <v>1.05</v>
       </c>
       <c r="G3">
-        <v>0.822</v>
+        <v>0.82</v>
       </c>
       <c r="H3">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4">
@@ -2591,19 +2591,19 @@
         <v>1.6</v>
       </c>
       <c r="E4">
-        <v>1.116</v>
+        <v>1.12</v>
       </c>
       <c r="F4">
-        <v>2.293</v>
+        <v>2.29</v>
       </c>
       <c r="G4">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="H4">
-        <v>0.034</v>
+        <v>0.03</v>
       </c>
       <c r="I4">
-        <v>0.184</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="5">
@@ -2623,22 +2623,22 @@
         </is>
       </c>
       <c r="D5">
-        <v>199.991</v>
+        <v>199.99</v>
       </c>
       <c r="E5">
-        <v>0.097</v>
+        <v>0.1</v>
       </c>
       <c r="F5">
-        <v>413598.977</v>
+        <v>413598.98</v>
       </c>
       <c r="G5">
-        <v>0.174</v>
+        <v>0.17</v>
       </c>
       <c r="H5">
-        <v>15.172</v>
+        <v>15.17</v>
       </c>
       <c r="I5">
-        <v>3.895</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="6">
@@ -2658,22 +2658,22 @@
         </is>
       </c>
       <c r="D6">
-        <v>650.573</v>
+        <v>650.5700000000001</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>29702356334.421</v>
+        <v>29702356334.42</v>
       </c>
       <c r="G6">
-        <v>0.472</v>
+        <v>0.47</v>
       </c>
       <c r="H6">
-        <v>80.97199999999999</v>
+        <v>80.97</v>
       </c>
       <c r="I6">
-        <v>8.997999999999999</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -2693,22 +2693,22 @@
         </is>
       </c>
       <c r="D7">
-        <v>134.358</v>
+        <v>134.36</v>
       </c>
       <c r="E7">
-        <v>0.032</v>
+        <v>0.03</v>
       </c>
       <c r="F7">
-        <v>572454.446</v>
+        <v>572454.45</v>
       </c>
       <c r="G7">
         <v>0.25</v>
       </c>
       <c r="H7">
-        <v>18.181</v>
+        <v>18.18</v>
       </c>
       <c r="I7">
-        <v>4.264</v>
+        <v>4.26</v>
       </c>
     </row>
     <row r="8">
@@ -2728,22 +2728,22 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.287</v>
+        <v>0.29</v>
       </c>
       <c r="E8">
         <v>0.11</v>
       </c>
       <c r="F8">
-        <v>0.753</v>
+        <v>0.75</v>
       </c>
       <c r="G8">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="H8">
-        <v>0.242</v>
+        <v>0.24</v>
       </c>
       <c r="I8">
-        <v>0.492</v>
+        <v>0.49</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -2766,22 +2766,22 @@
         </is>
       </c>
       <c r="D9">
-        <v>1.005</v>
+        <v>1.01</v>
       </c>
       <c r="E9">
-        <v>0.961</v>
+        <v>0.96</v>
       </c>
       <c r="F9">
-        <v>1.052</v>
+        <v>1.05</v>
       </c>
       <c r="G9">
-        <v>0.822</v>
+        <v>0.82</v>
       </c>
       <c r="H9">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -2807,19 +2807,19 @@
         <v>1.6</v>
       </c>
       <c r="E10">
-        <v>1.116</v>
+        <v>1.12</v>
       </c>
       <c r="F10">
-        <v>2.293</v>
+        <v>2.29</v>
       </c>
       <c r="G10">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="H10">
-        <v>0.034</v>
+        <v>0.03</v>
       </c>
       <c r="I10">
-        <v>0.184</v>
+        <v>0.18</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -2842,22 +2842,22 @@
         </is>
       </c>
       <c r="D11">
-        <v>199.991</v>
+        <v>199.99</v>
       </c>
       <c r="E11">
-        <v>0.097</v>
+        <v>0.1</v>
       </c>
       <c r="F11">
         <v>411722.56</v>
       </c>
       <c r="G11">
-        <v>0.174</v>
+        <v>0.17</v>
       </c>
       <c r="H11">
-        <v>15.154</v>
+        <v>15.15</v>
       </c>
       <c r="I11">
-        <v>3.893</v>
+        <v>3.89</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2880,22 +2880,22 @@
         </is>
       </c>
       <c r="D12">
-        <v>650.573</v>
+        <v>650.5700000000001</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>28984793312.418</v>
+        <v>28984793312.42</v>
       </c>
       <c r="G12">
-        <v>0.471</v>
+        <v>0.47</v>
       </c>
       <c r="H12">
-        <v>80.748</v>
+        <v>80.75</v>
       </c>
       <c r="I12">
-        <v>8.986000000000001</v>
+        <v>8.99</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -2918,13 +2918,13 @@
         </is>
       </c>
       <c r="D13">
-        <v>134.358</v>
+        <v>134.36</v>
       </c>
       <c r="E13">
-        <v>0.032</v>
+        <v>0.03</v>
       </c>
       <c r="F13">
-        <v>569710.819</v>
+        <v>569710.8199999999</v>
       </c>
       <c r="G13">
         <v>0.25</v>
@@ -2933,7 +2933,7 @@
         <v>18.16</v>
       </c>
       <c r="I13">
-        <v>4.261</v>
+        <v>4.26</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -2956,25 +2956,25 @@
         </is>
       </c>
       <c r="D14">
-        <v>0.324</v>
+        <v>0.32</v>
       </c>
       <c r="E14">
-        <v>0.141</v>
+        <v>0.14</v>
       </c>
       <c r="F14">
-        <v>0.746</v>
+        <v>0.75</v>
       </c>
       <c r="G14">
-        <v>0.008</v>
+        <v>0.01</v>
       </c>
       <c r="H14">
-        <v>0.181</v>
+        <v>0.18</v>
       </c>
       <c r="I14">
-        <v>0.425</v>
+        <v>0.43</v>
       </c>
       <c r="J14">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="15">
@@ -2994,25 +2994,25 @@
         </is>
       </c>
       <c r="D15">
-        <v>1.005</v>
+        <v>1.01</v>
       </c>
       <c r="E15">
-        <v>0.974</v>
+        <v>0.97</v>
       </c>
       <c r="F15">
-        <v>1.037</v>
+        <v>1.04</v>
       </c>
       <c r="G15">
-        <v>0.757</v>
+        <v>0.76</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0.016</v>
+        <v>0.02</v>
       </c>
       <c r="J15">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="16">
@@ -3032,25 +3032,25 @@
         </is>
       </c>
       <c r="D16">
-        <v>1.581</v>
+        <v>1.58</v>
       </c>
       <c r="E16">
-        <v>1.175</v>
+        <v>1.18</v>
       </c>
       <c r="F16">
-        <v>2.126</v>
+        <v>2.13</v>
       </c>
       <c r="G16">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
       <c r="I16">
-        <v>0.151</v>
+        <v>0.15</v>
       </c>
       <c r="J16">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="17">
@@ -3070,13 +3070,13 @@
         </is>
       </c>
       <c r="D17">
-        <v>379.979</v>
+        <v>379.98</v>
       </c>
       <c r="E17">
-        <v>2.529</v>
+        <v>2.53</v>
       </c>
       <c r="F17">
-        <v>57093.841</v>
+        <v>57093.84</v>
       </c>
       <c r="G17">
         <v>0.02</v>
@@ -3085,10 +3085,10 @@
         <v>6.54</v>
       </c>
       <c r="I17">
-        <v>2.557</v>
+        <v>2.56</v>
       </c>
       <c r="J17">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="18">
@@ -3108,25 +3108,25 @@
         </is>
       </c>
       <c r="D18">
-        <v>178.817</v>
+        <v>178.82</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>1232714156.037</v>
+        <v>1232714156.04</v>
       </c>
       <c r="G18">
-        <v>0.519</v>
+        <v>0.52</v>
       </c>
       <c r="H18">
-        <v>64.54300000000001</v>
+        <v>64.54000000000001</v>
       </c>
       <c r="I18">
-        <v>8.034000000000001</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="J18">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="19">
@@ -3146,25 +3146,25 @@
         </is>
       </c>
       <c r="D19">
-        <v>65.102</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="E19">
-        <v>0.07199999999999999</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F19">
-        <v>58732.464</v>
+        <v>58732.46</v>
       </c>
       <c r="G19">
-        <v>0.229</v>
+        <v>0.23</v>
       </c>
       <c r="H19">
-        <v>12.054</v>
+        <v>12.05</v>
       </c>
       <c r="I19">
-        <v>3.472</v>
+        <v>3.47</v>
       </c>
       <c r="J19">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
   </sheetData>
@@ -3249,22 +3249,22 @@
         </is>
       </c>
       <c r="D2">
-        <v>-1.139</v>
+        <v>-1.14</v>
       </c>
       <c r="E2">
-        <v>-2.109</v>
+        <v>-2.11</v>
       </c>
       <c r="F2">
-        <v>-0.168</v>
+        <v>-0.17</v>
       </c>
       <c r="G2">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="H2">
-        <v>0.245</v>
+        <v>0.25</v>
       </c>
       <c r="I2">
-        <v>0.495</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -3284,22 +3284,22 @@
         </is>
       </c>
       <c r="D3">
-        <v>-0.835</v>
+        <v>-0.84</v>
       </c>
       <c r="E3">
-        <v>-1.703</v>
+        <v>-1.7</v>
       </c>
       <c r="F3">
-        <v>0.032</v>
+        <v>0.03</v>
       </c>
       <c r="G3">
-        <v>0.059</v>
+        <v>0.06</v>
       </c>
       <c r="H3">
-        <v>0.196</v>
+        <v>0.2</v>
       </c>
       <c r="I3">
-        <v>0.443</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="4">
@@ -3319,22 +3319,22 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>-0.042</v>
+        <v>-0.04</v>
       </c>
       <c r="F4">
-        <v>0.049</v>
+        <v>0.05</v>
       </c>
       <c r="G4">
-        <v>0.889</v>
+        <v>0.89</v>
       </c>
       <c r="H4">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="5">
@@ -3357,19 +3357,19 @@
         <v>0.46</v>
       </c>
       <c r="E5">
-        <v>0.099</v>
+        <v>0.1</v>
       </c>
       <c r="F5">
-        <v>0.821</v>
+        <v>0.82</v>
       </c>
       <c r="G5">
-        <v>0.013</v>
+        <v>0.01</v>
       </c>
       <c r="H5">
-        <v>0.034</v>
+        <v>0.03</v>
       </c>
       <c r="I5">
-        <v>0.184</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="6">
@@ -3389,22 +3389,22 @@
         </is>
       </c>
       <c r="D6">
-        <v>5.363</v>
+        <v>5.36</v>
       </c>
       <c r="E6">
-        <v>-2.283</v>
+        <v>-2.28</v>
       </c>
       <c r="F6">
-        <v>13.009</v>
+        <v>13.01</v>
       </c>
       <c r="G6">
-        <v>0.169</v>
+        <v>0.17</v>
       </c>
       <c r="H6">
-        <v>15.217</v>
+        <v>15.22</v>
       </c>
       <c r="I6">
-        <v>3.901</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="7">
@@ -3424,22 +3424,22 @@
         </is>
       </c>
       <c r="D7">
-        <v>6.578</v>
+        <v>6.58</v>
       </c>
       <c r="E7">
-        <v>-11.019</v>
+        <v>-11.02</v>
       </c>
       <c r="F7">
-        <v>24.176</v>
+        <v>24.18</v>
       </c>
       <c r="G7">
-        <v>0.464</v>
+        <v>0.46</v>
       </c>
       <c r="H7">
-        <v>80.614</v>
+        <v>80.61</v>
       </c>
       <c r="I7">
-        <v>8.978999999999999</v>
+        <v>8.98</v>
       </c>
     </row>
     <row r="8">
@@ -3459,22 +3459,22 @@
         </is>
       </c>
       <c r="D8">
-        <v>4.884</v>
+        <v>4.88</v>
       </c>
       <c r="E8">
-        <v>-3.453</v>
+        <v>-3.45</v>
       </c>
       <c r="F8">
         <v>13.22</v>
       </c>
       <c r="G8">
-        <v>0.251</v>
+        <v>0.25</v>
       </c>
       <c r="H8">
-        <v>18.092</v>
+        <v>18.09</v>
       </c>
       <c r="I8">
-        <v>4.253</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="9">
@@ -3494,22 +3494,22 @@
         </is>
       </c>
       <c r="D9">
-        <v>-1.139</v>
+        <v>-1.14</v>
       </c>
       <c r="E9">
-        <v>-2.109</v>
+        <v>-2.11</v>
       </c>
       <c r="F9">
-        <v>-0.169</v>
+        <v>-0.17</v>
       </c>
       <c r="G9">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="H9">
-        <v>0.245</v>
+        <v>0.24</v>
       </c>
       <c r="I9">
-        <v>0.495</v>
+        <v>0.49</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -3532,22 +3532,22 @@
         </is>
       </c>
       <c r="D10">
-        <v>-0.835</v>
+        <v>-0.84</v>
       </c>
       <c r="E10">
-        <v>-1.703</v>
+        <v>-1.7</v>
       </c>
       <c r="F10">
-        <v>0.032</v>
+        <v>0.03</v>
       </c>
       <c r="G10">
-        <v>0.059</v>
+        <v>0.06</v>
       </c>
       <c r="H10">
-        <v>0.196</v>
+        <v>0.2</v>
       </c>
       <c r="I10">
-        <v>0.443</v>
+        <v>0.44</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -3570,22 +3570,22 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>-0.042</v>
+        <v>-0.04</v>
       </c>
       <c r="F11">
-        <v>0.049</v>
+        <v>0.05</v>
       </c>
       <c r="G11">
-        <v>0.889</v>
+        <v>0.89</v>
       </c>
       <c r="H11">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -3611,19 +3611,19 @@
         <v>0.46</v>
       </c>
       <c r="E12">
-        <v>0.099</v>
+        <v>0.1</v>
       </c>
       <c r="F12">
-        <v>0.821</v>
+        <v>0.82</v>
       </c>
       <c r="G12">
-        <v>0.013</v>
+        <v>0.01</v>
       </c>
       <c r="H12">
-        <v>0.034</v>
+        <v>0.03</v>
       </c>
       <c r="I12">
-        <v>0.184</v>
+        <v>0.18</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -3646,22 +3646,22 @@
         </is>
       </c>
       <c r="D13">
-        <v>5.363</v>
+        <v>5.36</v>
       </c>
       <c r="E13">
-        <v>-2.277</v>
+        <v>-2.28</v>
       </c>
       <c r="F13">
-        <v>13.003</v>
+        <v>13</v>
       </c>
       <c r="G13">
-        <v>0.169</v>
+        <v>0.17</v>
       </c>
       <c r="H13">
-        <v>15.194</v>
+        <v>15.19</v>
       </c>
       <c r="I13">
-        <v>3.898</v>
+        <v>3.9</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -3684,22 +3684,22 @@
         </is>
       </c>
       <c r="D14">
-        <v>6.578</v>
+        <v>6.58</v>
       </c>
       <c r="E14">
         <v>-10.95</v>
       </c>
       <c r="F14">
-        <v>24.106</v>
+        <v>24.11</v>
       </c>
       <c r="G14">
-        <v>0.462</v>
+        <v>0.46</v>
       </c>
       <c r="H14">
-        <v>79.977</v>
+        <v>79.98</v>
       </c>
       <c r="I14">
-        <v>8.943</v>
+        <v>8.94</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -3722,22 +3722,22 @@
         </is>
       </c>
       <c r="D15">
-        <v>4.884</v>
+        <v>4.88</v>
       </c>
       <c r="E15">
-        <v>-3.439</v>
+        <v>-3.44</v>
       </c>
       <c r="F15">
-        <v>13.207</v>
+        <v>13.21</v>
       </c>
       <c r="G15">
         <v>0.25</v>
       </c>
       <c r="H15">
-        <v>18.033</v>
+        <v>18.03</v>
       </c>
       <c r="I15">
-        <v>4.247</v>
+        <v>4.25</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -3760,25 +3760,25 @@
         </is>
       </c>
       <c r="D16">
-        <v>-1.068</v>
+        <v>-1.07</v>
       </c>
       <c r="E16">
-        <v>-1.928</v>
+        <v>-1.93</v>
       </c>
       <c r="F16">
-        <v>-0.207</v>
+        <v>-0.21</v>
       </c>
       <c r="G16">
-        <v>0.015</v>
+        <v>0.02</v>
       </c>
       <c r="H16">
-        <v>0.193</v>
+        <v>0.19</v>
       </c>
       <c r="I16">
-        <v>0.439</v>
+        <v>0.44</v>
       </c>
       <c r="J16">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="17">
@@ -3798,25 +3798,25 @@
         </is>
       </c>
       <c r="D17">
-        <v>-0.843</v>
+        <v>-0.84</v>
       </c>
       <c r="E17">
-        <v>-1.726</v>
+        <v>-1.73</v>
       </c>
       <c r="F17">
         <v>0.04</v>
       </c>
       <c r="G17">
-        <v>0.061</v>
+        <v>0.06</v>
       </c>
       <c r="H17">
-        <v>0.203</v>
+        <v>0.2</v>
       </c>
       <c r="I17">
-        <v>0.451</v>
+        <v>0.45</v>
       </c>
       <c r="J17">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="18">
@@ -3836,25 +3836,25 @@
         </is>
       </c>
       <c r="D18">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>-0.029</v>
+        <v>-0.03</v>
       </c>
       <c r="F18">
-        <v>0.036</v>
+        <v>0.04</v>
       </c>
       <c r="G18">
-        <v>0.843</v>
+        <v>0.84</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0.016</v>
+        <v>0.02</v>
       </c>
       <c r="J18">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="19">
@@ -3874,25 +3874,25 @@
         </is>
       </c>
       <c r="D19">
-        <v>0.447</v>
+        <v>0.45</v>
       </c>
       <c r="E19">
-        <v>0.145</v>
+        <v>0.14</v>
       </c>
       <c r="F19">
         <v>0.75</v>
       </c>
       <c r="G19">
-        <v>0.004</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>0.024</v>
+        <v>0.02</v>
       </c>
       <c r="I19">
-        <v>0.154</v>
+        <v>0.15</v>
       </c>
       <c r="J19">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="20">
@@ -3912,25 +3912,25 @@
         </is>
       </c>
       <c r="D20">
-        <v>5.814</v>
+        <v>5.81</v>
       </c>
       <c r="E20">
-        <v>0.798</v>
+        <v>0.8</v>
       </c>
       <c r="F20">
-        <v>10.831</v>
+        <v>10.83</v>
       </c>
       <c r="G20">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
       <c r="H20">
-        <v>6.551</v>
+        <v>6.55</v>
       </c>
       <c r="I20">
-        <v>2.559</v>
+        <v>2.56</v>
       </c>
       <c r="J20">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="21">
@@ -3950,25 +3950,25 @@
         </is>
       </c>
       <c r="D21">
-        <v>5.686</v>
+        <v>5.69</v>
       </c>
       <c r="E21">
-        <v>-10.048</v>
+        <v>-10.05</v>
       </c>
       <c r="F21">
-        <v>21.421</v>
+        <v>21.42</v>
       </c>
       <c r="G21">
-        <v>0.479</v>
+        <v>0.48</v>
       </c>
       <c r="H21">
-        <v>64.447</v>
+        <v>64.45</v>
       </c>
       <c r="I21">
-        <v>8.028</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="J21">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="22">
@@ -3988,25 +3988,25 @@
         </is>
       </c>
       <c r="D22">
-        <v>4.503</v>
+        <v>4.5</v>
       </c>
       <c r="E22">
-        <v>-2.194</v>
+        <v>-2.19</v>
       </c>
       <c r="F22">
-        <v>11.199</v>
+        <v>11.2</v>
       </c>
       <c r="G22">
-        <v>0.188</v>
+        <v>0.19</v>
       </c>
       <c r="H22">
-        <v>11.672</v>
+        <v>11.67</v>
       </c>
       <c r="I22">
-        <v>3.416</v>
+        <v>3.42</v>
       </c>
       <c r="J22">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
   </sheetData>
@@ -4094,19 +4094,19 @@
         <v>0.32</v>
       </c>
       <c r="E2">
-        <v>0.121</v>
+        <v>0.12</v>
       </c>
       <c r="F2">
-        <v>0.845</v>
+        <v>0.85</v>
       </c>
       <c r="G2">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="H2">
-        <v>0.245</v>
+        <v>0.25</v>
       </c>
       <c r="I2">
-        <v>0.495</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -4126,22 +4126,22 @@
         </is>
       </c>
       <c r="D3">
-        <v>0.434</v>
+        <v>0.43</v>
       </c>
       <c r="E3">
-        <v>0.182</v>
+        <v>0.18</v>
       </c>
       <c r="F3">
-        <v>1.032</v>
+        <v>1.03</v>
       </c>
       <c r="G3">
-        <v>0.059</v>
+        <v>0.06</v>
       </c>
       <c r="H3">
-        <v>0.196</v>
+        <v>0.2</v>
       </c>
       <c r="I3">
-        <v>0.443</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="4">
@@ -4161,22 +4161,22 @@
         </is>
       </c>
       <c r="D4">
-        <v>1.003</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.959</v>
+        <v>0.96</v>
       </c>
       <c r="F4">
         <v>1.05</v>
       </c>
       <c r="G4">
-        <v>0.889</v>
+        <v>0.89</v>
       </c>
       <c r="H4">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="5">
@@ -4196,22 +4196,22 @@
         </is>
       </c>
       <c r="D5">
-        <v>1.583</v>
+        <v>1.58</v>
       </c>
       <c r="E5">
-        <v>1.104</v>
+        <v>1.1</v>
       </c>
       <c r="F5">
-        <v>2.272</v>
+        <v>2.27</v>
       </c>
       <c r="G5">
-        <v>0.013</v>
+        <v>0.01</v>
       </c>
       <c r="H5">
-        <v>0.034</v>
+        <v>0.03</v>
       </c>
       <c r="I5">
-        <v>0.184</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="6">
@@ -4234,19 +4234,19 @@
         <v>213.39</v>
       </c>
       <c r="E6">
-        <v>0.102</v>
+        <v>0.1</v>
       </c>
       <c r="F6">
-        <v>446300.371</v>
+        <v>446300.37</v>
       </c>
       <c r="G6">
-        <v>0.169</v>
+        <v>0.17</v>
       </c>
       <c r="H6">
-        <v>15.217</v>
+        <v>15.22</v>
       </c>
       <c r="I6">
-        <v>3.901</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="7">
@@ -4266,22 +4266,22 @@
         </is>
       </c>
       <c r="D7">
-        <v>719.298</v>
+        <v>719.3</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>31583436568.721</v>
+        <v>31583436568.72</v>
       </c>
       <c r="G7">
-        <v>0.464</v>
+        <v>0.46</v>
       </c>
       <c r="H7">
-        <v>80.614</v>
+        <v>80.61</v>
       </c>
       <c r="I7">
-        <v>8.978999999999999</v>
+        <v>8.98</v>
       </c>
     </row>
     <row r="8">
@@ -4301,22 +4301,22 @@
         </is>
       </c>
       <c r="D8">
-        <v>132.096</v>
+        <v>132.1</v>
       </c>
       <c r="E8">
-        <v>0.032</v>
+        <v>0.03</v>
       </c>
       <c r="F8">
-        <v>551381.067</v>
+        <v>551381.0699999999</v>
       </c>
       <c r="G8">
-        <v>0.251</v>
+        <v>0.25</v>
       </c>
       <c r="H8">
-        <v>18.092</v>
+        <v>18.09</v>
       </c>
       <c r="I8">
-        <v>4.253</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="9">
@@ -4339,19 +4339,19 @@
         <v>0.32</v>
       </c>
       <c r="E9">
-        <v>0.121</v>
+        <v>0.12</v>
       </c>
       <c r="F9">
-        <v>0.845</v>
+        <v>0.84</v>
       </c>
       <c r="G9">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="H9">
-        <v>0.245</v>
+        <v>0.24</v>
       </c>
       <c r="I9">
-        <v>0.495</v>
+        <v>0.49</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -4374,22 +4374,22 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.434</v>
+        <v>0.43</v>
       </c>
       <c r="E10">
-        <v>0.182</v>
+        <v>0.18</v>
       </c>
       <c r="F10">
-        <v>1.032</v>
+        <v>1.03</v>
       </c>
       <c r="G10">
-        <v>0.059</v>
+        <v>0.06</v>
       </c>
       <c r="H10">
-        <v>0.196</v>
+        <v>0.2</v>
       </c>
       <c r="I10">
-        <v>0.443</v>
+        <v>0.44</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -4412,22 +4412,22 @@
         </is>
       </c>
       <c r="D11">
-        <v>1.003</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0.959</v>
+        <v>0.96</v>
       </c>
       <c r="F11">
         <v>1.05</v>
       </c>
       <c r="G11">
-        <v>0.889</v>
+        <v>0.89</v>
       </c>
       <c r="H11">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -4450,22 +4450,22 @@
         </is>
       </c>
       <c r="D12">
-        <v>1.583</v>
+        <v>1.58</v>
       </c>
       <c r="E12">
-        <v>1.104</v>
+        <v>1.1</v>
       </c>
       <c r="F12">
-        <v>2.272</v>
+        <v>2.27</v>
       </c>
       <c r="G12">
-        <v>0.013</v>
+        <v>0.01</v>
       </c>
       <c r="H12">
-        <v>0.034</v>
+        <v>0.03</v>
       </c>
       <c r="I12">
-        <v>0.184</v>
+        <v>0.18</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -4491,19 +4491,19 @@
         <v>213.39</v>
       </c>
       <c r="E13">
-        <v>0.103</v>
+        <v>0.1</v>
       </c>
       <c r="F13">
-        <v>443738.775</v>
+        <v>443738.78</v>
       </c>
       <c r="G13">
-        <v>0.169</v>
+        <v>0.17</v>
       </c>
       <c r="H13">
-        <v>15.194</v>
+        <v>15.19</v>
       </c>
       <c r="I13">
-        <v>3.898</v>
+        <v>3.9</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -4526,22 +4526,22 @@
         </is>
       </c>
       <c r="D14">
-        <v>719.298</v>
+        <v>719.3</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>29456601165.252</v>
+        <v>29456601165.25</v>
       </c>
       <c r="G14">
-        <v>0.462</v>
+        <v>0.46</v>
       </c>
       <c r="H14">
-        <v>79.977</v>
+        <v>79.98</v>
       </c>
       <c r="I14">
-        <v>8.943</v>
+        <v>8.94</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -4564,22 +4564,22 @@
         </is>
       </c>
       <c r="D15">
-        <v>132.096</v>
+        <v>132.1</v>
       </c>
       <c r="E15">
-        <v>0.032</v>
+        <v>0.03</v>
       </c>
       <c r="F15">
-        <v>543918.144</v>
+        <v>543918.14</v>
       </c>
       <c r="G15">
         <v>0.25</v>
       </c>
       <c r="H15">
-        <v>18.033</v>
+        <v>18.03</v>
       </c>
       <c r="I15">
-        <v>4.247</v>
+        <v>4.25</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -4602,25 +4602,25 @@
         </is>
       </c>
       <c r="D16">
-        <v>0.344</v>
+        <v>0.34</v>
       </c>
       <c r="E16">
-        <v>0.145</v>
+        <v>0.15</v>
       </c>
       <c r="F16">
-        <v>0.8129999999999999</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="G16">
-        <v>0.015</v>
+        <v>0.02</v>
       </c>
       <c r="H16">
-        <v>0.193</v>
+        <v>0.19</v>
       </c>
       <c r="I16">
-        <v>0.439</v>
+        <v>0.44</v>
       </c>
       <c r="J16">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="17">
@@ -4643,22 +4643,22 @@
         <v>0.43</v>
       </c>
       <c r="E17">
-        <v>0.178</v>
+        <v>0.18</v>
       </c>
       <c r="F17">
-        <v>1.041</v>
+        <v>1.04</v>
       </c>
       <c r="G17">
-        <v>0.061</v>
+        <v>0.06</v>
       </c>
       <c r="H17">
-        <v>0.203</v>
+        <v>0.2</v>
       </c>
       <c r="I17">
-        <v>0.451</v>
+        <v>0.45</v>
       </c>
       <c r="J17">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="18">
@@ -4678,25 +4678,25 @@
         </is>
       </c>
       <c r="D18">
-        <v>1.003</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0.971</v>
+        <v>0.97</v>
       </c>
       <c r="F18">
-        <v>1.036</v>
+        <v>1.04</v>
       </c>
       <c r="G18">
-        <v>0.843</v>
+        <v>0.84</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0.016</v>
+        <v>0.02</v>
       </c>
       <c r="J18">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="19">
@@ -4716,25 +4716,25 @@
         </is>
       </c>
       <c r="D19">
-        <v>1.564</v>
+        <v>1.56</v>
       </c>
       <c r="E19">
-        <v>1.156</v>
+        <v>1.16</v>
       </c>
       <c r="F19">
-        <v>2.117</v>
+        <v>2.12</v>
       </c>
       <c r="G19">
-        <v>0.004</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>0.024</v>
+        <v>0.02</v>
       </c>
       <c r="I19">
-        <v>0.154</v>
+        <v>0.15</v>
       </c>
       <c r="J19">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="20">
@@ -4754,25 +4754,25 @@
         </is>
       </c>
       <c r="D20">
-        <v>335.043</v>
+        <v>335.04</v>
       </c>
       <c r="E20">
-        <v>2.221</v>
+        <v>2.22</v>
       </c>
       <c r="F20">
-        <v>50553.098</v>
+        <v>50553.1</v>
       </c>
       <c r="G20">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
       <c r="H20">
-        <v>6.551</v>
+        <v>6.55</v>
       </c>
       <c r="I20">
-        <v>2.559</v>
+        <v>2.56</v>
       </c>
       <c r="J20">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="21">
@@ -4801,16 +4801,16 @@
         <v>2008996524.39</v>
       </c>
       <c r="G21">
-        <v>0.479</v>
+        <v>0.48</v>
       </c>
       <c r="H21">
-        <v>64.447</v>
+        <v>64.45</v>
       </c>
       <c r="I21">
-        <v>8.028</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="J21">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="22">
@@ -4830,25 +4830,25 @@
         </is>
       </c>
       <c r="D22">
-        <v>90.251</v>
+        <v>90.25</v>
       </c>
       <c r="E22">
-        <v>0.112</v>
+        <v>0.11</v>
       </c>
       <c r="F22">
-        <v>73037.799</v>
+        <v>73037.8</v>
       </c>
       <c r="G22">
-        <v>0.188</v>
+        <v>0.19</v>
       </c>
       <c r="H22">
-        <v>11.672</v>
+        <v>11.67</v>
       </c>
       <c r="I22">
-        <v>3.416</v>
+        <v>3.42</v>
       </c>
       <c r="J22">
-        <v>-0.003</v>
+        <v>-0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating all results based on new covariate selection criteria (use same covariates for all models and only do backwards selection for LRT)
</commit_message>
<xml_diff>
--- a/3_Results/32_ResultsVMMC/vmmc_individual_adjusted.xlsx
+++ b/3_Results/32_ResultsVMMC/vmmc_individual_adjusted.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Y1_ik ~ T_k + age + marital_status + education + monthly_income + alcohol_weekly + partners_12mos + prop_began_infected + prop_male + prop_vlsupp</t>
+          <t>Y1_ik ~ T_k + age + marital_status + education + alcohol_weekly + partners_12mos + prop_began_infected + prop_male + prop_vlsupp</t>
         </is>
       </c>
     </row>
@@ -468,7 +468,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Y1_ik ~ T_k + alcohol_weekly + partners_12mos + prop_began_infected</t>
+          <t>Y1_ik ~ T_k + age + marital_status + education + alcohol_weekly + partners_12mos + prop_began_infected + prop_male + prop_vlsupp</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Y1_ik ~ T_k + X1_ik + age + marital_status + education + monthly_income + alcohol_weekly + partners_12mos + prop_began_infected + prop_male + prop_vlsupp</t>
+          <t>Y1_ik ~ T_k + X1_ik + age + marital_status + education + alcohol_weekly + partners_12mos + prop_began_infected + prop_male + prop_vlsupp</t>
         </is>
       </c>
     </row>
@@ -492,7 +492,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Y1_ik ~ T_k + X1_ik + alcohol_weekly + partners_12mos + prop_began_infected</t>
+          <t>Y1_ik ~ T_k + X1_ik + age + marital_status + education + alcohol_weekly + partners_12mos + prop_began_infected + prop_male + prop_vlsupp</t>
         </is>
       </c>
     </row>
@@ -569,20 +569,20 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>-0.94 (-1.78, -0.1)</t>
+          <t>-1.21 (-2.19, -0.24)</t>
         </is>
       </c>
       <c r="E2">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="F2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="H2">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -603,20 +603,20 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>-0.84 (-1.68, 0)</t>
+          <t>-1.12 (-2.1, -0.14)</t>
         </is>
       </c>
       <c r="E3">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="H3">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4">
@@ -637,7 +637,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-0.1 (-1.48, 1.28)</t>
+          <t>-0.09 (-1.47, 1.29)</t>
         </is>
       </c>
       <c r="E4">
@@ -647,7 +647,7 @@
         <v>0.5</v>
       </c>
       <c r="H4">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5">
@@ -668,7 +668,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-0.1 (NA, NA)</t>
+          <t>-0.09 (NA, NA)</t>
         </is>
       </c>
     </row>
@@ -690,17 +690,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.09 (-1.04, 1.21)</t>
+          <t>0.08 (-1.02, 1.17)</t>
         </is>
       </c>
       <c r="E6">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="G6">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
       <c r="H6">
-        <v>0.57</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -721,7 +721,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.11 (NA, NA)</t>
+          <t>0.08 (NA, NA)</t>
         </is>
       </c>
     </row>
@@ -798,20 +798,20 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.39 (0.17, 0.91)</t>
+          <t>0.3 (0.11, 0.79)</t>
         </is>
       </c>
       <c r="E2">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="F2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="H2">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -832,20 +832,20 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.43 (0.19, 1)</t>
+          <t>0.33 (0.12, 0.87)</t>
         </is>
       </c>
       <c r="E3">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="H3">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4">
@@ -866,7 +866,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.9 (0.23, 3.61)</t>
+          <t>0.91 (0.23, 3.63)</t>
         </is>
       </c>
       <c r="E4">
@@ -876,7 +876,7 @@
         <v>0.5</v>
       </c>
       <c r="H4">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5">
@@ -919,17 +919,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.09 (-1.04, 1.21)</t>
+          <t>0.08 (-1.02, 1.17)</t>
         </is>
       </c>
       <c r="E6">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="G6">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
       <c r="H6">
-        <v>0.57</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -950,7 +950,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.11 (NA, NA)</t>
+          <t>0.08 (NA, NA)</t>
         </is>
       </c>
     </row>
@@ -961,7 +961,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1017,20 +1017,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-0.94 (-1.78, -0.1)</t>
+          <t>-1.21 (-2.19, -0.24)</t>
         </is>
       </c>
       <c r="D2">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="G2">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -1041,25 +1041,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>alcohol_weekly</t>
+          <t>age</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.17 (-0.08, 0.43)</t>
+          <t>0.02 (-0.03, 0.08)</t>
         </is>
       </c>
       <c r="D3">
-        <v>0.17</v>
+        <v>0.37</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4">
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>partners_12mos</t>
+          <t>marital_statusMarried</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.4 (0.04, 0.77)</t>
+          <t>-7.19 (-192444.7, 192430.31)</t>
         </is>
       </c>
       <c r="D4">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.03</v>
+        <v>9640138065.84</v>
       </c>
       <c r="G4">
-        <v>0.19</v>
+        <v>98184.2</v>
       </c>
     </row>
     <row r="5">
@@ -1099,25 +1099,315 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>marital_statusSingle/never married</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>16.68 (-24333.3, 24366.65)</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>154347965.07</v>
+      </c>
+      <c r="G5">
+        <v>12423.69</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>marital_statusWidowed</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>-4.69 (-418865.97, 418856.59)</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>45671391190.95</v>
+      </c>
+      <c r="G6">
+        <v>213708.66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>educationJunior secondary</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.85 (-0.41, 2.1)</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0.19</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.41</v>
+      </c>
+      <c r="G7">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>educationNon-formal</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.91 (-0.98, 2.8)</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.35</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.93</v>
+      </c>
+      <c r="G8">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>educationPrimary</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>-0.64 (-2.95, 1.67)</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.59</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1.39</v>
+      </c>
+      <c r="G9">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>educationSenior secondary</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.05 (-1.48, 1.59)</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.61</v>
+      </c>
+      <c r="G10">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>alcohol_weekly</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.13 (-0.12, 0.39)</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.31</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.02</v>
+      </c>
+      <c r="G11">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>partners_12mos</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.43 (0.05, 0.8)</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.02</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0.04</v>
+      </c>
+      <c r="G12">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>prop_began_infected</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>7.07 (1.11, 13.04)</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>0.02</v>
-      </c>
-      <c r="E5">
-        <v>0.01</v>
-      </c>
-      <c r="F5">
-        <v>9.25</v>
-      </c>
-      <c r="G5">
-        <v>3.04</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>4.45 (-3.2, 12.11)</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.25</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>15.26</v>
+      </c>
+      <c r="G13">
+        <v>3.91</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>prop_male</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>6.24 (-11.63, 24.1)</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.49</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>83.09</v>
+      </c>
+      <c r="G14">
+        <v>9.119999999999999</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>prop_vlsupp</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>5.69 (-2.86, 14.25)</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>0.19</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>19.05</v>
+      </c>
+      <c r="G15">
+        <v>4.36</v>
       </c>
     </row>
   </sheetData>
@@ -1127,7 +1417,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1183,20 +1473,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.39 (0.17, 0.91)</t>
+          <t>0.3 (0.11, 0.79)</t>
         </is>
       </c>
       <c r="D2">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="G2">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -1207,25 +1497,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>alcohol_weekly</t>
+          <t>age</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.19 (0.93, 1.53)</t>
+          <t>1.03 (0.97, 1.08)</t>
         </is>
       </c>
       <c r="D3">
-        <v>0.17</v>
+        <v>0.37</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4">
@@ -1236,25 +1526,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>partners_12mos</t>
+          <t>marital_statusMarried</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.5 (1.04, 2.16)</t>
+          <t>0 (0, Inf)</t>
         </is>
       </c>
       <c r="D4">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.03</v>
+        <v>9640138065.84</v>
       </c>
       <c r="G4">
-        <v>0.19</v>
+        <v>98184.2</v>
       </c>
     </row>
     <row r="5">
@@ -1265,25 +1555,315 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>marital_statusSingle/never married</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>17493449.33 (0, Inf)</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>154347965.07</v>
+      </c>
+      <c r="G5">
+        <v>12423.69</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>marital_statusWidowed</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.01 (0, Inf)</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>45671391190.95</v>
+      </c>
+      <c r="G6">
+        <v>213708.66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>educationJunior secondary</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2.33 (0.66, 8.2)</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0.19</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.41</v>
+      </c>
+      <c r="G7">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>educationNon-formal</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2.48 (0.38, 16.42)</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.35</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.93</v>
+      </c>
+      <c r="G8">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>educationPrimary</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.53 (0.05, 5.29)</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.59</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1.39</v>
+      </c>
+      <c r="G9">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>educationSenior secondary</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1.06 (0.23, 4.88)</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.61</v>
+      </c>
+      <c r="G10">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>alcohol_weekly</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1.14 (0.88, 1.48)</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.31</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.02</v>
+      </c>
+      <c r="G11">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>partners_12mos</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1.54 (1.06, 2.23)</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.02</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0.04</v>
+      </c>
+      <c r="G12">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>prop_began_infected</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1181.89 (3.04, 458765.96)</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>0.02</v>
-      </c>
-      <c r="E5">
-        <v>0.01</v>
-      </c>
-      <c r="F5">
-        <v>9.25</v>
-      </c>
-      <c r="G5">
-        <v>3.04</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>85.89 (0.04, 181521.49)</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.25</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>15.26</v>
+      </c>
+      <c r="G13">
+        <v>3.91</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>prop_male</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>511.53 (0, 29384422254.67)</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.49</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>83.09</v>
+      </c>
+      <c r="G14">
+        <v>9.119999999999999</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Total Effects Model</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>prop_vlsupp</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>296.82 (0.06, 1539448.48)</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>0.19</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>19.05</v>
+      </c>
+      <c r="G15">
+        <v>4.36</v>
       </c>
     </row>
   </sheetData>
@@ -1293,7 +1873,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1349,20 +1929,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-0.84 (-1.68, 0)</t>
+          <t>-1.12 (-2.1, -0.14)</t>
         </is>
       </c>
       <c r="D2">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="G2">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -1378,14 +1958,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-0.81 (-1.68, 0.06)</t>
+          <t>-0.84 (-1.71, 0.03)</t>
         </is>
       </c>
       <c r="D3">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0.2</v>
@@ -1402,25 +1982,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>alcohol_weekly</t>
+          <t>age</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.16 (-0.09, 0.41)</t>
+          <t>0.02 (-0.03, 0.08)</t>
         </is>
       </c>
       <c r="D4">
-        <v>0.21</v>
+        <v>0.44</v>
       </c>
       <c r="E4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5">
@@ -1431,25 +2011,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>partners_12mos</t>
+          <t>marital_statusMarried</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.4 (0.03, 0.76)</t>
+          <t>-13.92 (-5749421.72, 5749393.89)</t>
         </is>
       </c>
       <c r="D5">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.04</v>
+        <v>8604983589036.44</v>
       </c>
       <c r="G5">
-        <v>0.19</v>
+        <v>2933425.23</v>
       </c>
     </row>
     <row r="6">
@@ -1460,25 +2040,315 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>marital_statusSingle/never married</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>16.77 (-23986.6, 24020.13)</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>149985141.05</v>
+      </c>
+      <c r="G6">
+        <v>12246.84</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>marital_statusWidowed</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>-19.09 (-65765501.71, 65765463.54)</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1125900056827765</v>
+      </c>
+      <c r="G7">
+        <v>33554434.23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>educationJunior secondary</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.84 (-0.42, 2.1)</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.19</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.41</v>
+      </c>
+      <c r="G8">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>educationNon-formal</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.91 (-0.98, 2.8)</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.34</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.93</v>
+      </c>
+      <c r="G9">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>educationPrimary</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>-0.69 (-3, 1.62)</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1.39</v>
+      </c>
+      <c r="G10">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>educationSenior secondary</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>-0.02 (-1.56, 1.51)</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.98</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.61</v>
+      </c>
+      <c r="G11">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>alcohol_weekly</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.12 (-0.13, 0.38)</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.35</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0.02</v>
+      </c>
+      <c r="G12">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>partners_12mos</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.43 (0.05, 0.81)</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.03</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0.04</v>
+      </c>
+      <c r="G13">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>prop_began_infected</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>7.12 (1.2, 13.04)</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>0.02</v>
-      </c>
-      <c r="E6">
-        <v>0.01</v>
-      </c>
-      <c r="F6">
-        <v>9.130000000000001</v>
-      </c>
-      <c r="G6">
-        <v>3.02</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>4.44 (-3.22, 12.1)</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.26</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>15.28</v>
+      </c>
+      <c r="G14">
+        <v>3.91</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>prop_male</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>6.51 (-11.32, 24.34)</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>0.47</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>82.78</v>
+      </c>
+      <c r="G15">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>prop_vlsupp</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>5.78 (-2.77, 14.32)</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>0.19</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>18.99</v>
+      </c>
+      <c r="G16">
+        <v>4.36</v>
       </c>
     </row>
   </sheetData>
@@ -1488,7 +2358,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1544,20 +2414,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.43 (0.19, 1)</t>
+          <t>0.33 (0.12, 0.87)</t>
         </is>
       </c>
       <c r="D2">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="G2">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -1573,14 +2443,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.44 (0.19, 1.06)</t>
+          <t>0.43 (0.18, 1.03)</t>
         </is>
       </c>
       <c r="D3">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0.2</v>
@@ -1597,25 +2467,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>alcohol_weekly</t>
+          <t>age</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.17 (0.91, 1.51)</t>
+          <t>1.02 (0.97, 1.08)</t>
         </is>
       </c>
       <c r="D4">
-        <v>0.21</v>
+        <v>0.44</v>
       </c>
       <c r="E4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5">
@@ -1626,25 +2496,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>partners_12mos</t>
+          <t>marital_statusMarried</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.49 (1.03, 2.15)</t>
+          <t>0 (0, Inf)</t>
         </is>
       </c>
       <c r="D5">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.04</v>
+        <v>8604983589036.44</v>
       </c>
       <c r="G5">
-        <v>0.19</v>
+        <v>2933425.23</v>
       </c>
     </row>
     <row r="6">
@@ -1655,25 +2525,315 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>marital_statusSingle/never married</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>19104448.61 (0, Inf)</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>149985141.05</v>
+      </c>
+      <c r="G6">
+        <v>12246.84</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>marital_statusWidowed</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0 (0, Inf)</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1125900056827765</v>
+      </c>
+      <c r="G7">
+        <v>33554434.23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>educationJunior secondary</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2.31 (0.66, 8.13)</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.19</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.41</v>
+      </c>
+      <c r="G8">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>educationNon-formal</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2.49 (0.38, 16.52)</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.34</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.93</v>
+      </c>
+      <c r="G9">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>educationPrimary</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.5 (0.05, 5.08)</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1.39</v>
+      </c>
+      <c r="G10">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>educationSenior secondary</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.98 (0.21, 4.53)</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.98</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.61</v>
+      </c>
+      <c r="G11">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>alcohol_weekly</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1.13 (0.87, 1.46)</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.35</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0.02</v>
+      </c>
+      <c r="G12">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>partners_12mos</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1.54 (1.05, 2.25)</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.03</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0.04</v>
+      </c>
+      <c r="G13">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>prop_began_infected</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1233.45 (3.31, 460238.31)</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>0.02</v>
-      </c>
-      <c r="E6">
-        <v>0.01</v>
-      </c>
-      <c r="F6">
-        <v>9.130000000000001</v>
-      </c>
-      <c r="G6">
-        <v>3.02</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>84.73 (0.04, 180058.84)</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.26</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>15.28</v>
+      </c>
+      <c r="G14">
+        <v>3.91</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>prop_male</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>672.77 (0, 37363370516.25)</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>0.47</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>82.78</v>
+      </c>
+      <c r="G15">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Direct Effects Model</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>prop_vlsupp</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>322.38 (0.06, 1652667.9)</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>0.19</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>18.99</v>
+      </c>
+      <c r="G16">
+        <v>4.36</v>
       </c>
     </row>
   </sheetData>
@@ -1683,7 +2843,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1712,16 +2872,6 @@
           <t>age</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>marital_status</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>T_k</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1729,16 +2879,6 @@
           <t>marital_status</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>monthly_income</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>alcohol_weekly</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1746,74 +2886,37 @@
           <t>education</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>age</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>partners_12mos</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>monthly_income</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>prop_male</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>prop_began_infected</t>
+          <t>alcohol_weekly</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>alcohol_weekly</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>education</t>
+          <t>partners_12mos</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>partners_12mos</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>prop_vlsupp</t>
+          <t>prop_began_infected</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>prop_began_infected</t>
+          <t>prop_male</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
-        <is>
-          <t>prop_male</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
         <is>
           <t>prop_vlsupp</t>
         </is>

</xml_diff>